<commit_message>
Fix SQL error due to comma (') in imported values
Version 1.8
</commit_message>
<xml_diff>
--- a/tests/Students_RosarioSIS_test.xlsx
+++ b/tests/Students_RosarioSIS_test.xlsx
@@ -62,7 +62,7 @@
     <t xml:space="preserve">Meryl</t>
   </si>
   <si>
-    <t xml:space="preserve">Streep</t>
+    <t xml:space="preserve">Streep’</t>
   </si>
   <si>
     <t xml:space="preserve">Female</t>
@@ -275,17 +275,17 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.2793522267206"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>

</xml_diff>